<commit_message>
Renamed Parsing on Performance Chart to Parse
</commit_message>
<xml_diff>
--- a/Doc/performance.xlsx
+++ b/Doc/performance.xlsx
@@ -30,9 +30,6 @@
     <t>ToString</t>
   </si>
   <si>
-    <t>Parsing</t>
-  </si>
-  <si>
     <t>Enum.Parse (Names)</t>
   </si>
   <si>
@@ -106,6 +103,9 @@
   </si>
   <si>
     <t>UnsafeEnums.Parse (Decimal Values)</t>
+  </si>
+  <si>
+    <t>Parse</t>
   </si>
 </sst>
 </file>
@@ -502,7 +502,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Parsing</c:v>
+                  <c:v>Parse</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1756,8 +1756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1781,21 +1781,21 @@
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="H1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>991</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" s="2">
         <f>B16</f>
@@ -1816,13 +1816,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>515</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" s="2">
         <f>B14</f>
@@ -1843,7 +1843,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <v>368</v>
@@ -1867,7 +1867,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>1017</v>
@@ -1891,7 +1891,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>697</v>
@@ -1899,7 +1899,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7">
         <v>538</v>
@@ -1907,7 +1907,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>992</v>
@@ -1915,7 +1915,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>55</v>
@@ -1923,7 +1923,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>20</v>
@@ -1931,7 +1931,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>74</v>
@@ -1939,7 +1939,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>83</v>
@@ -1947,7 +1947,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>43</v>
@@ -1955,7 +1955,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14">
         <v>1053</v>
@@ -1963,7 +1963,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15">
         <v>183</v>
@@ -1971,7 +1971,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>20</v>
@@ -1979,7 +1979,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17">
         <v>24</v>
@@ -1987,7 +1987,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>931</v>
@@ -1995,7 +1995,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19">
         <v>244</v>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20">
         <v>1085</v>
@@ -2011,7 +2011,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>2395</v>
@@ -2019,7 +2019,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22">
         <v>178</v>
@@ -2027,7 +2027,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23">
         <v>103</v>

</xml_diff>

<commit_message>
Fixed font size on HasFlag performance graph
</commit_message>
<xml_diff>
--- a/Doc/performance.xlsx
+++ b/Doc/performance.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\Source\Repos\Enums.NET\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brinkleyt\Source\Repos\Enums.NET\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="1200" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -111,7 +111,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0&quot;ms&quot;"/>
   </numFmts>
@@ -166,7 +166,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -223,6 +223,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -321,8 +322,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -370,7 +372,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-930E-4993-A756-32E3459B6CDB}"/>
             </c:ext>
@@ -438,8 +440,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -487,7 +490,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3F28-49BB-8332-18C94E060697}"/>
             </c:ext>
@@ -555,8 +558,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -604,7 +608,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-3F28-49BB-8332-18C94E060697}"/>
             </c:ext>
@@ -649,7 +653,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -672,8 +676,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -721,7 +726,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-FCB9-404E-91DF-EC83070EA9E3}"/>
             </c:ext>
@@ -738,11 +743,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1831528647"/>
-        <c:axId val="2070664071"/>
+        <c:axId val="196838160"/>
+        <c:axId val="196838552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1831528647"/>
+        <c:axId val="196838160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -785,7 +790,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2070664071"/>
+        <c:crossAx val="196838552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -793,7 +798,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2070664071"/>
+        <c:axId val="196838552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -803,7 +808,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1831528647"/>
+        <c:crossAx val="196838160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -817,6 +822,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1446,7 +1452,7 @@
         <xdr:cNvPr id="4" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{918EA447-6805-4A76-A5C4-358C6502A744}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{918EA447-6805-4A76-A5C4-358C6502A744}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1757,7 +1763,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>